<commit_message>
Update BunkerPrices at 2025-03-19 14:59
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV3"/>
+  <dimension ref="A1:AV4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,12 +563,12 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>Montevideo</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>New York</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
@@ -756,10 +756,10 @@
         <v>536</v>
       </c>
       <c r="Y2" t="n">
+        <v>534</v>
+      </c>
+      <c r="Z2" t="n">
         <v>552</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>534</v>
       </c>
       <c r="AA2" t="n">
         <v>509</v>
@@ -902,10 +902,10 @@
         <v>529</v>
       </c>
       <c r="Y3" t="n">
+        <v>535</v>
+      </c>
+      <c r="Z3" t="n">
         <v>553</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>535</v>
       </c>
       <c r="AA3" t="n">
         <v>503</v>
@@ -928,7 +928,7 @@
       <c r="AG3" t="n">
         <v>494</v>
       </c>
-      <c r="AH3" s="3" t="n">
+      <c r="AH3" s="2" t="n">
         <v>45733</v>
       </c>
       <c r="AI3" t="n">
@@ -972,6 +972,152 @@
       </c>
       <c r="AV3" t="n">
         <v>638</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>577</v>
+      </c>
+      <c r="B4" t="n">
+        <v>646</v>
+      </c>
+      <c r="C4" t="n">
+        <v>499</v>
+      </c>
+      <c r="D4" t="n">
+        <v>571</v>
+      </c>
+      <c r="E4" t="n">
+        <v>620</v>
+      </c>
+      <c r="F4" t="n">
+        <v>645</v>
+      </c>
+      <c r="G4" t="n">
+        <v>502</v>
+      </c>
+      <c r="H4" t="n">
+        <v>516</v>
+      </c>
+      <c r="I4" t="n">
+        <v>563</v>
+      </c>
+      <c r="J4" t="n">
+        <v>520</v>
+      </c>
+      <c r="K4" t="n">
+        <v>582</v>
+      </c>
+      <c r="L4" t="n">
+        <v>516</v>
+      </c>
+      <c r="M4" t="n">
+        <v>532</v>
+      </c>
+      <c r="N4" t="n">
+        <v>883</v>
+      </c>
+      <c r="O4" t="n">
+        <v>578</v>
+      </c>
+      <c r="P4" t="n">
+        <v>526</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>502</v>
+      </c>
+      <c r="R4" t="n">
+        <v>530</v>
+      </c>
+      <c r="S4" t="n">
+        <v>605</v>
+      </c>
+      <c r="T4" t="n">
+        <v>646</v>
+      </c>
+      <c r="U4" t="n">
+        <v>588</v>
+      </c>
+      <c r="V4" t="n">
+        <v>490</v>
+      </c>
+      <c r="W4" t="n">
+        <v>560</v>
+      </c>
+      <c r="X4" t="n">
+        <v>528</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>530</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>552</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>502</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>543</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>584.5</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>515</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>514</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>527</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>490</v>
+      </c>
+      <c r="AH4" s="3" t="n">
+        <v>45730</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>505</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>537</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>520</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>750</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>646</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>610</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>500</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>640</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>760</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>515</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>499</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>566</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>578</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-03-20 01:56
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV6"/>
+  <dimension ref="A1:AV7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,12 +563,12 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
+          <t>Montevideo</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>New York</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Montevideo</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
@@ -756,10 +756,10 @@
         <v>536</v>
       </c>
       <c r="Y2" t="n">
+        <v>552</v>
+      </c>
+      <c r="Z2" t="n">
         <v>534</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>552</v>
       </c>
       <c r="AA2" t="n">
         <v>509</v>
@@ -902,10 +902,10 @@
         <v>529</v>
       </c>
       <c r="Y3" t="n">
+        <v>553</v>
+      </c>
+      <c r="Z3" t="n">
         <v>535</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>553</v>
       </c>
       <c r="AA3" t="n">
         <v>503</v>
@@ -1048,10 +1048,10 @@
         <v>528</v>
       </c>
       <c r="Y4" t="n">
+        <v>552</v>
+      </c>
+      <c r="Z4" t="n">
         <v>530</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>552</v>
       </c>
       <c r="AA4" t="n">
         <v>502</v>
@@ -1194,10 +1194,10 @@
         <v>530</v>
       </c>
       <c r="Y5" t="n">
+        <v>551</v>
+      </c>
+      <c r="Z5" t="n">
         <v>529</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>551</v>
       </c>
       <c r="AA5" t="n">
         <v>509</v>
@@ -1340,10 +1340,10 @@
         <v>515</v>
       </c>
       <c r="Y6" t="n">
+        <v>553</v>
+      </c>
+      <c r="Z6" t="n">
         <v>533</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>553</v>
       </c>
       <c r="AA6" t="n">
         <v>503</v>
@@ -1366,7 +1366,7 @@
       <c r="AG6" t="n">
         <v>490</v>
       </c>
-      <c r="AH6" s="3" t="n">
+      <c r="AH6" s="2" t="n">
         <v>45728</v>
       </c>
       <c r="AI6" t="n">
@@ -1410,6 +1410,152 @@
       </c>
       <c r="AV6" t="n">
         <v>639</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>560</v>
+      </c>
+      <c r="B7" t="n">
+        <v>640</v>
+      </c>
+      <c r="C7" t="n">
+        <v>492</v>
+      </c>
+      <c r="D7" t="n">
+        <v>545</v>
+      </c>
+      <c r="E7" t="n">
+        <v>645</v>
+      </c>
+      <c r="F7" t="n">
+        <v>639</v>
+      </c>
+      <c r="G7" t="n">
+        <v>498</v>
+      </c>
+      <c r="H7" t="n">
+        <v>532</v>
+      </c>
+      <c r="I7" t="n">
+        <v>561</v>
+      </c>
+      <c r="J7" t="n">
+        <v>515</v>
+      </c>
+      <c r="K7" t="n">
+        <v>575</v>
+      </c>
+      <c r="L7" t="n">
+        <v>505</v>
+      </c>
+      <c r="M7" t="n">
+        <v>533</v>
+      </c>
+      <c r="N7" t="n">
+        <v>880</v>
+      </c>
+      <c r="O7" t="n">
+        <v>583</v>
+      </c>
+      <c r="P7" t="n">
+        <v>523</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>498</v>
+      </c>
+      <c r="R7" t="n">
+        <v>537</v>
+      </c>
+      <c r="S7" t="n">
+        <v>582</v>
+      </c>
+      <c r="T7" t="n">
+        <v>653</v>
+      </c>
+      <c r="U7" t="n">
+        <v>589</v>
+      </c>
+      <c r="V7" t="n">
+        <v>485</v>
+      </c>
+      <c r="W7" t="n">
+        <v>545</v>
+      </c>
+      <c r="X7" t="n">
+        <v>530</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>548</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>531</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>498</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>542</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>585.5</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>508</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>510</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>529</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>485</v>
+      </c>
+      <c r="AH7" s="3" t="n">
+        <v>45735</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>502</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>546</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>515</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>742</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>656</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>617</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>500</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>628</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>752</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>511</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>492</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>554</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>569</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-03-28 02:23
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV10"/>
+  <dimension ref="A1:AV11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,122 +558,122 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
+          <t>Khor Fakkan</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
           <t>Petersburg</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Sydney</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Santos</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Istanbul</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>South Korea (West)</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Guayaquil</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Vancouver</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Buenos Aires</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Las Palmas</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Valparaiso</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Durban</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Novorossiisk</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>New Orleans</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Singapore</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Kuwait</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Zhoushan</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Rotterdam</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Algeciras</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Antwerp</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Guayaquil</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Vancouver</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Buenos Aires</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Las Palmas</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Cartagena</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Valparaiso</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Durban</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Novorossiisk</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>New Orleans</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Singapore</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Lisbon</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Kuwait</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Zhoushan</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Rotterdam</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Algeciras</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>Japan</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>Khor Fakkan</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
@@ -753,22 +753,22 @@
         <v>498</v>
       </c>
       <c r="X2" t="n">
+        <v>509</v>
+      </c>
+      <c r="Y2" t="n">
         <v>545</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Z2" t="n">
         <v>752</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AA2" t="n">
         <v>536</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>560</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>520</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>495</v>
       </c>
       <c r="AD2" t="n">
         <v>639</v>
@@ -822,7 +822,7 @@
         <v>550</v>
       </c>
       <c r="AU2" t="n">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="AV2" t="n">
         <v>534</v>
@@ -899,22 +899,22 @@
         <v>498</v>
       </c>
       <c r="X3" t="n">
+        <v>503</v>
+      </c>
+      <c r="Y3" t="n">
         <v>565</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="Z3" t="n">
         <v>746</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AA3" t="n">
         <v>529</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>566</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>514</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>494</v>
       </c>
       <c r="AD3" t="n">
         <v>640</v>
@@ -968,7 +968,7 @@
         <v>543</v>
       </c>
       <c r="AU3" t="n">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="AV3" t="n">
         <v>535</v>
@@ -1045,22 +1045,22 @@
         <v>499</v>
       </c>
       <c r="X4" t="n">
+        <v>502</v>
+      </c>
+      <c r="Y4" t="n">
         <v>560</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Z4" t="n">
         <v>750</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AA4" t="n">
         <v>528</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>577</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>514</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>490</v>
       </c>
       <c r="AD4" t="n">
         <v>646</v>
@@ -1114,7 +1114,7 @@
         <v>543</v>
       </c>
       <c r="AU4" t="n">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="AV4" t="n">
         <v>530</v>
@@ -1191,22 +1191,22 @@
         <v>502</v>
       </c>
       <c r="X5" t="n">
+        <v>509</v>
+      </c>
+      <c r="Y5" t="n">
         <v>555</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Z5" t="n">
         <v>765</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AA5" t="n">
         <v>530</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>577</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>515</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>490</v>
       </c>
       <c r="AD5" t="n">
         <v>644</v>
@@ -1260,7 +1260,7 @@
         <v>550</v>
       </c>
       <c r="AU5" t="n">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="AV5" t="n">
         <v>529</v>
@@ -1337,22 +1337,22 @@
         <v>495</v>
       </c>
       <c r="X6" t="n">
+        <v>503</v>
+      </c>
+      <c r="Y6" t="n">
         <v>550</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="Z6" t="n">
         <v>758</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AA6" t="n">
         <v>515</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AB6" t="n">
         <v>570</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>520</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>490</v>
       </c>
       <c r="AD6" t="n">
         <v>648</v>
@@ -1406,7 +1406,7 @@
         <v>545</v>
       </c>
       <c r="AU6" t="n">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="AV6" t="n">
         <v>533</v>
@@ -1483,22 +1483,22 @@
         <v>492</v>
       </c>
       <c r="X7" t="n">
+        <v>498</v>
+      </c>
+      <c r="Y7" t="n">
         <v>545</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="Z7" t="n">
         <v>742</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AA7" t="n">
         <v>530</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AB7" t="n">
         <v>560</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>510</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>485</v>
       </c>
       <c r="AD7" t="n">
         <v>640</v>
@@ -1552,7 +1552,7 @@
         <v>542</v>
       </c>
       <c r="AU7" t="n">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="AV7" t="n">
         <v>531</v>
@@ -1629,22 +1629,22 @@
         <v>498</v>
       </c>
       <c r="X8" t="n">
+        <v>504</v>
+      </c>
+      <c r="Y8" t="n">
         <v>560</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="Z8" t="n">
         <v>748</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AA8" t="n">
         <v>535</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AB8" t="n">
         <v>558</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AC8" t="n">
         <v>514</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>494</v>
       </c>
       <c r="AD8" t="n">
         <v>643</v>
@@ -1698,7 +1698,7 @@
         <v>548</v>
       </c>
       <c r="AU8" t="n">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="AV8" t="n">
         <v>534</v>
@@ -1775,22 +1775,22 @@
         <v>501</v>
       </c>
       <c r="X9" t="n">
+        <v>508</v>
+      </c>
+      <c r="Y9" t="n">
         <v>560</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="Z9" t="n">
         <v>753</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AA9" t="n">
         <v>538</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AB9" t="n">
         <v>558</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AC9" t="n">
         <v>520</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>490</v>
       </c>
       <c r="AD9" t="n">
         <v>651</v>
@@ -1844,7 +1844,7 @@
         <v>551</v>
       </c>
       <c r="AU9" t="n">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="AV9" t="n">
         <v>542</v>
@@ -1905,7 +1905,7 @@
       <c r="R10" t="n">
         <v>664</v>
       </c>
-      <c r="S10" s="3" t="n">
+      <c r="S10" s="2" t="n">
         <v>45740</v>
       </c>
       <c r="T10" t="n">
@@ -1921,22 +1921,22 @@
         <v>501</v>
       </c>
       <c r="X10" t="n">
+        <v>508</v>
+      </c>
+      <c r="Y10" t="n">
         <v>555</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="Z10" t="n">
         <v>753</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AA10" t="n">
         <v>535</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AB10" t="n">
         <v>565</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AC10" t="n">
         <v>524</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>493</v>
       </c>
       <c r="AD10" t="n">
         <v>652</v>
@@ -1990,10 +1990,156 @@
         <v>550</v>
       </c>
       <c r="AU10" t="n">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="AV10" t="n">
         <v>544</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>520</v>
+      </c>
+      <c r="B11" t="n">
+        <v>572</v>
+      </c>
+      <c r="C11" t="n">
+        <v>535</v>
+      </c>
+      <c r="D11" t="n">
+        <v>517</v>
+      </c>
+      <c r="E11" t="n">
+        <v>650</v>
+      </c>
+      <c r="F11" t="n">
+        <v>522</v>
+      </c>
+      <c r="G11" t="n">
+        <v>650</v>
+      </c>
+      <c r="H11" t="n">
+        <v>659</v>
+      </c>
+      <c r="I11" t="n">
+        <v>582</v>
+      </c>
+      <c r="J11" t="n">
+        <v>520</v>
+      </c>
+      <c r="K11" t="n">
+        <v>562</v>
+      </c>
+      <c r="L11" t="n">
+        <v>513</v>
+      </c>
+      <c r="M11" t="n">
+        <v>585</v>
+      </c>
+      <c r="N11" t="n">
+        <v>523</v>
+      </c>
+      <c r="O11" t="n">
+        <v>645</v>
+      </c>
+      <c r="P11" t="n">
+        <v>767</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>570</v>
+      </c>
+      <c r="R11" t="n">
+        <v>665</v>
+      </c>
+      <c r="S11" s="3" t="n">
+        <v>45741</v>
+      </c>
+      <c r="T11" t="n">
+        <v>585</v>
+      </c>
+      <c r="U11" t="n">
+        <v>592</v>
+      </c>
+      <c r="V11" t="n">
+        <v>607</v>
+      </c>
+      <c r="W11" t="n">
+        <v>508</v>
+      </c>
+      <c r="X11" t="n">
+        <v>513</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>555</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>757</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>538</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>574</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>527</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>651</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>603.5</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>562</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>528</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>573</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>882</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>650</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>507</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>623</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>547</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>517</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>535</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>513</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>508</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>490</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>522</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>552</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>490</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-03-28 06:08
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV13"/>
+  <dimension ref="A1:AV14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2343,7 +2343,7 @@
       <c r="R13" t="n">
         <v>655</v>
       </c>
-      <c r="S13" s="3" t="n">
+      <c r="S13" s="2" t="n">
         <v>45734</v>
       </c>
       <c r="T13" t="n">
@@ -2432,6 +2432,152 @@
       </c>
       <c r="AV13" t="n">
         <v>534</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>521</v>
+      </c>
+      <c r="B14" t="n">
+        <v>572</v>
+      </c>
+      <c r="C14" t="n">
+        <v>536</v>
+      </c>
+      <c r="D14" t="n">
+        <v>522</v>
+      </c>
+      <c r="E14" t="n">
+        <v>652</v>
+      </c>
+      <c r="F14" t="n">
+        <v>530</v>
+      </c>
+      <c r="G14" t="n">
+        <v>629</v>
+      </c>
+      <c r="H14" t="n">
+        <v>665</v>
+      </c>
+      <c r="I14" t="n">
+        <v>565</v>
+      </c>
+      <c r="J14" t="n">
+        <v>526</v>
+      </c>
+      <c r="K14" t="n">
+        <v>568</v>
+      </c>
+      <c r="L14" t="n">
+        <v>519</v>
+      </c>
+      <c r="M14" t="n">
+        <v>580</v>
+      </c>
+      <c r="N14" t="n">
+        <v>527</v>
+      </c>
+      <c r="O14" t="n">
+        <v>651</v>
+      </c>
+      <c r="P14" t="n">
+        <v>772</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>560</v>
+      </c>
+      <c r="R14" t="n">
+        <v>668</v>
+      </c>
+      <c r="S14" s="3" t="n">
+        <v>45743</v>
+      </c>
+      <c r="T14" t="n">
+        <v>592</v>
+      </c>
+      <c r="U14" t="n">
+        <v>600</v>
+      </c>
+      <c r="V14" t="n">
+        <v>610</v>
+      </c>
+      <c r="W14" t="n">
+        <v>515</v>
+      </c>
+      <c r="X14" t="n">
+        <v>519</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>550</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>762</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>542</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>573</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>526</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>653</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>606.5</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>579</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>533</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>576</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>884</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>650</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>510</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>629</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>546</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>521</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>535</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>519</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>515</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>497</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>530</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>552</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>497</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-04 13:20
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV16"/>
+  <dimension ref="A1:AV17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,12 +578,12 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
+          <t>Montreal*</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
           <t>Hong Kong</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Montreal*</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
@@ -765,10 +765,10 @@
         <v>509</v>
       </c>
       <c r="AB2" t="n">
+        <v>655</v>
+      </c>
+      <c r="AC2" t="n">
         <v>515</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>655</v>
       </c>
       <c r="AD2" t="n">
         <v>622</v>
@@ -911,10 +911,10 @@
         <v>503</v>
       </c>
       <c r="AB3" t="n">
+        <v>645</v>
+      </c>
+      <c r="AC3" t="n">
         <v>512</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>645</v>
       </c>
       <c r="AD3" t="n">
         <v>616</v>
@@ -1057,10 +1057,10 @@
         <v>502</v>
       </c>
       <c r="AB4" t="n">
+        <v>646</v>
+      </c>
+      <c r="AC4" t="n">
         <v>515</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>646</v>
       </c>
       <c r="AD4" t="n">
         <v>610</v>
@@ -1203,10 +1203,10 @@
         <v>509</v>
       </c>
       <c r="AB5" t="n">
+        <v>644</v>
+      </c>
+      <c r="AC5" t="n">
         <v>520</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>644</v>
       </c>
       <c r="AD5" t="n">
         <v>613</v>
@@ -1349,10 +1349,10 @@
         <v>503</v>
       </c>
       <c r="AB6" t="n">
+        <v>649</v>
+      </c>
+      <c r="AC6" t="n">
         <v>520</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>649</v>
       </c>
       <c r="AD6" t="n">
         <v>610</v>
@@ -1495,10 +1495,10 @@
         <v>498</v>
       </c>
       <c r="AB7" t="n">
+        <v>656</v>
+      </c>
+      <c r="AC7" t="n">
         <v>508</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>656</v>
       </c>
       <c r="AD7" t="n">
         <v>617</v>
@@ -1641,10 +1641,10 @@
         <v>504</v>
       </c>
       <c r="AB8" t="n">
+        <v>660</v>
+      </c>
+      <c r="AC8" t="n">
         <v>515</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>660</v>
       </c>
       <c r="AD8" t="n">
         <v>623</v>
@@ -1787,10 +1787,10 @@
         <v>508</v>
       </c>
       <c r="AB9" t="n">
+        <v>661</v>
+      </c>
+      <c r="AC9" t="n">
         <v>517</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>661</v>
       </c>
       <c r="AD9" t="n">
         <v>621</v>
@@ -1933,10 +1933,10 @@
         <v>508</v>
       </c>
       <c r="AB10" t="n">
+        <v>664</v>
+      </c>
+      <c r="AC10" t="n">
         <v>518</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>664</v>
       </c>
       <c r="AD10" t="n">
         <v>622</v>
@@ -2079,10 +2079,10 @@
         <v>513</v>
       </c>
       <c r="AB11" t="n">
+        <v>665</v>
+      </c>
+      <c r="AC11" t="n">
         <v>523</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>665</v>
       </c>
       <c r="AD11" t="n">
         <v>623</v>
@@ -2225,10 +2225,10 @@
         <v>513</v>
       </c>
       <c r="AB12" t="n">
+        <v>667</v>
+      </c>
+      <c r="AC12" t="n">
         <v>521</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>667</v>
       </c>
       <c r="AD12" t="n">
         <v>625</v>
@@ -2371,10 +2371,10 @@
         <v>509</v>
       </c>
       <c r="AB13" t="n">
+        <v>655</v>
+      </c>
+      <c r="AC13" t="n">
         <v>515</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>655</v>
       </c>
       <c r="AD13" t="n">
         <v>622</v>
@@ -2517,10 +2517,10 @@
         <v>519</v>
       </c>
       <c r="AB14" t="n">
+        <v>668</v>
+      </c>
+      <c r="AC14" t="n">
         <v>527</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>668</v>
       </c>
       <c r="AD14" t="n">
         <v>629</v>
@@ -2663,10 +2663,10 @@
         <v>523</v>
       </c>
       <c r="AB15" t="n">
+        <v>667</v>
+      </c>
+      <c r="AC15" t="n">
         <v>528</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>667</v>
       </c>
       <c r="AD15" t="n">
         <v>619</v>
@@ -2739,7 +2739,7 @@
       <c r="D16" t="n">
         <v>525</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="2" t="n">
         <v>45748</v>
       </c>
       <c r="F16" t="n">
@@ -2809,10 +2809,10 @@
         <v>533</v>
       </c>
       <c r="AB16" t="n">
+        <v>673</v>
+      </c>
+      <c r="AC16" t="n">
         <v>538</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>673</v>
       </c>
       <c r="AD16" t="n">
         <v>628</v>
@@ -2869,6 +2869,152 @@
         <v>785</v>
       </c>
       <c r="AV16" t="n">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>565</v>
+      </c>
+      <c r="B17" t="n">
+        <v>585</v>
+      </c>
+      <c r="C17" t="n">
+        <v>878</v>
+      </c>
+      <c r="D17" t="n">
+        <v>532</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>45749</v>
+      </c>
+      <c r="F17" t="n">
+        <v>534</v>
+      </c>
+      <c r="G17" t="n">
+        <v>535</v>
+      </c>
+      <c r="H17" t="n">
+        <v>574</v>
+      </c>
+      <c r="I17" t="n">
+        <v>584</v>
+      </c>
+      <c r="J17" t="n">
+        <v>552</v>
+      </c>
+      <c r="K17" t="n">
+        <v>572</v>
+      </c>
+      <c r="L17" t="n">
+        <v>595</v>
+      </c>
+      <c r="M17" t="n">
+        <v>502</v>
+      </c>
+      <c r="N17" t="n">
+        <v>600</v>
+      </c>
+      <c r="O17" t="n">
+        <v>656</v>
+      </c>
+      <c r="P17" t="n">
+        <v>535</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>584</v>
+      </c>
+      <c r="R17" t="n">
+        <v>532</v>
+      </c>
+      <c r="S17" t="n">
+        <v>564</v>
+      </c>
+      <c r="T17" t="n">
+        <v>668</v>
+      </c>
+      <c r="U17" t="n">
+        <v>623</v>
+      </c>
+      <c r="V17" t="n">
+        <v>603</v>
+      </c>
+      <c r="W17" t="n">
+        <v>625</v>
+      </c>
+      <c r="X17" t="n">
+        <v>534</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>577</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>778</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>535</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>675</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>540</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>629</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>532</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>565</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>515</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>667</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>535</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>559</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>619.5</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>645</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>545</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>537</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>580</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>663</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>525</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>556</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>502</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>542</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>788</v>
+      </c>
+      <c r="AV17" t="n">
         <v>530</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-04 13:21
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV17"/>
+  <dimension ref="A1:AV18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,12 +578,12 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
+          <t>Hong Kong</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
           <t>Montreal*</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Hong Kong</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
@@ -765,10 +765,10 @@
         <v>509</v>
       </c>
       <c r="AB2" t="n">
+        <v>515</v>
+      </c>
+      <c r="AC2" t="n">
         <v>655</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>515</v>
       </c>
       <c r="AD2" t="n">
         <v>622</v>
@@ -911,10 +911,10 @@
         <v>503</v>
       </c>
       <c r="AB3" t="n">
+        <v>512</v>
+      </c>
+      <c r="AC3" t="n">
         <v>645</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>512</v>
       </c>
       <c r="AD3" t="n">
         <v>616</v>
@@ -1057,10 +1057,10 @@
         <v>502</v>
       </c>
       <c r="AB4" t="n">
+        <v>515</v>
+      </c>
+      <c r="AC4" t="n">
         <v>646</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>515</v>
       </c>
       <c r="AD4" t="n">
         <v>610</v>
@@ -1203,10 +1203,10 @@
         <v>509</v>
       </c>
       <c r="AB5" t="n">
+        <v>520</v>
+      </c>
+      <c r="AC5" t="n">
         <v>644</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>520</v>
       </c>
       <c r="AD5" t="n">
         <v>613</v>
@@ -1349,10 +1349,10 @@
         <v>503</v>
       </c>
       <c r="AB6" t="n">
+        <v>520</v>
+      </c>
+      <c r="AC6" t="n">
         <v>649</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>520</v>
       </c>
       <c r="AD6" t="n">
         <v>610</v>
@@ -1495,10 +1495,10 @@
         <v>498</v>
       </c>
       <c r="AB7" t="n">
+        <v>508</v>
+      </c>
+      <c r="AC7" t="n">
         <v>656</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>508</v>
       </c>
       <c r="AD7" t="n">
         <v>617</v>
@@ -1641,10 +1641,10 @@
         <v>504</v>
       </c>
       <c r="AB8" t="n">
+        <v>515</v>
+      </c>
+      <c r="AC8" t="n">
         <v>660</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>515</v>
       </c>
       <c r="AD8" t="n">
         <v>623</v>
@@ -1787,10 +1787,10 @@
         <v>508</v>
       </c>
       <c r="AB9" t="n">
+        <v>517</v>
+      </c>
+      <c r="AC9" t="n">
         <v>661</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>517</v>
       </c>
       <c r="AD9" t="n">
         <v>621</v>
@@ -1933,10 +1933,10 @@
         <v>508</v>
       </c>
       <c r="AB10" t="n">
+        <v>518</v>
+      </c>
+      <c r="AC10" t="n">
         <v>664</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>518</v>
       </c>
       <c r="AD10" t="n">
         <v>622</v>
@@ -2079,10 +2079,10 @@
         <v>513</v>
       </c>
       <c r="AB11" t="n">
+        <v>523</v>
+      </c>
+      <c r="AC11" t="n">
         <v>665</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>523</v>
       </c>
       <c r="AD11" t="n">
         <v>623</v>
@@ -2225,10 +2225,10 @@
         <v>513</v>
       </c>
       <c r="AB12" t="n">
+        <v>521</v>
+      </c>
+      <c r="AC12" t="n">
         <v>667</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>521</v>
       </c>
       <c r="AD12" t="n">
         <v>625</v>
@@ -2371,10 +2371,10 @@
         <v>509</v>
       </c>
       <c r="AB13" t="n">
+        <v>515</v>
+      </c>
+      <c r="AC13" t="n">
         <v>655</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>515</v>
       </c>
       <c r="AD13" t="n">
         <v>622</v>
@@ -2517,10 +2517,10 @@
         <v>519</v>
       </c>
       <c r="AB14" t="n">
+        <v>527</v>
+      </c>
+      <c r="AC14" t="n">
         <v>668</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>527</v>
       </c>
       <c r="AD14" t="n">
         <v>629</v>
@@ -2663,10 +2663,10 @@
         <v>523</v>
       </c>
       <c r="AB15" t="n">
+        <v>528</v>
+      </c>
+      <c r="AC15" t="n">
         <v>667</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>528</v>
       </c>
       <c r="AD15" t="n">
         <v>619</v>
@@ -2809,10 +2809,10 @@
         <v>533</v>
       </c>
       <c r="AB16" t="n">
+        <v>538</v>
+      </c>
+      <c r="AC16" t="n">
         <v>673</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>538</v>
       </c>
       <c r="AD16" t="n">
         <v>628</v>
@@ -2885,7 +2885,7 @@
       <c r="D17" t="n">
         <v>532</v>
       </c>
-      <c r="E17" s="3" t="n">
+      <c r="E17" s="2" t="n">
         <v>45749</v>
       </c>
       <c r="F17" t="n">
@@ -2955,10 +2955,10 @@
         <v>535</v>
       </c>
       <c r="AB17" t="n">
+        <v>540</v>
+      </c>
+      <c r="AC17" t="n">
         <v>675</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>540</v>
       </c>
       <c r="AD17" t="n">
         <v>629</v>
@@ -3016,6 +3016,152 @@
       </c>
       <c r="AV17" t="n">
         <v>530</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>544</v>
+      </c>
+      <c r="B18" t="n">
+        <v>570</v>
+      </c>
+      <c r="C18" t="n">
+        <v>872</v>
+      </c>
+      <c r="D18" t="n">
+        <v>522</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>45750</v>
+      </c>
+      <c r="F18" t="n">
+        <v>521</v>
+      </c>
+      <c r="G18" t="n">
+        <v>524</v>
+      </c>
+      <c r="H18" t="n">
+        <v>587.25</v>
+      </c>
+      <c r="I18" t="n">
+        <v>574</v>
+      </c>
+      <c r="J18" t="n">
+        <v>550</v>
+      </c>
+      <c r="K18" t="n">
+        <v>551</v>
+      </c>
+      <c r="L18" t="n">
+        <v>592</v>
+      </c>
+      <c r="M18" t="n">
+        <v>485</v>
+      </c>
+      <c r="N18" t="n">
+        <v>595</v>
+      </c>
+      <c r="O18" t="n">
+        <v>644</v>
+      </c>
+      <c r="P18" t="n">
+        <v>523</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>570</v>
+      </c>
+      <c r="R18" t="n">
+        <v>524</v>
+      </c>
+      <c r="S18" t="n">
+        <v>555</v>
+      </c>
+      <c r="T18" t="n">
+        <v>656</v>
+      </c>
+      <c r="U18" t="n">
+        <v>616</v>
+      </c>
+      <c r="V18" t="n">
+        <v>588</v>
+      </c>
+      <c r="W18" t="n">
+        <v>615</v>
+      </c>
+      <c r="X18" t="n">
+        <v>521</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>577</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>766</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>523</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>538</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>658</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>621</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>524</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>550</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>507</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>655</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>523</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>539</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>612.5</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>637</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>530</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>511</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>570</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>663</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>510</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>536</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>485</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>535</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>776</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-07 08:29
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV19"/>
+  <dimension ref="A1:AV20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3225,7 +3225,7 @@
       <c r="T19" t="n">
         <v>516</v>
       </c>
-      <c r="U19" s="3" t="n">
+      <c r="U19" s="2" t="n">
         <v>45751</v>
       </c>
       <c r="V19" t="n">
@@ -3307,6 +3307,122 @@
         <v>500</v>
       </c>
       <c r="AV19" t="n">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>552</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>560</v>
+      </c>
+      <c r="G20" t="n">
+        <v>613</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>543</v>
+      </c>
+      <c r="J20" t="n">
+        <v>546</v>
+      </c>
+      <c r="K20" t="n">
+        <v>540</v>
+      </c>
+      <c r="L20" t="n">
+        <v>580</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>515</v>
+      </c>
+      <c r="O20" t="n">
+        <v>501</v>
+      </c>
+      <c r="P20" t="n">
+        <v>654</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="n">
+        <v>546</v>
+      </c>
+      <c r="S20" t="n">
+        <v>523</v>
+      </c>
+      <c r="T20" t="n">
+        <v>567</v>
+      </c>
+      <c r="U20" s="3" t="n">
+        <v>45747</v>
+      </c>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="n">
+        <v>878</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>537</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>580</v>
+      </c>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="n">
+        <v>590</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>527</v>
+      </c>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="n">
+        <v>674</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>640</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>630</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>501</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>532</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>609.5</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>655</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>624</v>
+      </c>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="n">
+        <v>600</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>532</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>530</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>582</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>656</v>
+      </c>
+      <c r="AU20" t="inlineStr"/>
+      <c r="AV20" t="n">
         <v>660</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-14 02:41
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV21"/>
+  <dimension ref="A1:AV22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3499,7 +3499,7 @@
       <c r="X21" t="n">
         <v>495</v>
       </c>
-      <c r="Y21" s="3" t="n">
+      <c r="Y21" s="2" t="n">
         <v>45754</v>
       </c>
       <c r="Z21" t="n">
@@ -3569,6 +3569,152 @@
         <v>496</v>
       </c>
       <c r="AV21" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>565</v>
+      </c>
+      <c r="B22" t="n">
+        <v>474</v>
+      </c>
+      <c r="C22" t="n">
+        <v>450</v>
+      </c>
+      <c r="D22" t="n">
+        <v>522</v>
+      </c>
+      <c r="E22" t="n">
+        <v>515</v>
+      </c>
+      <c r="F22" t="n">
+        <v>520</v>
+      </c>
+      <c r="G22" t="n">
+        <v>474</v>
+      </c>
+      <c r="H22" t="n">
+        <v>570</v>
+      </c>
+      <c r="I22" t="n">
+        <v>490</v>
+      </c>
+      <c r="J22" t="n">
+        <v>450</v>
+      </c>
+      <c r="K22" t="n">
+        <v>571</v>
+      </c>
+      <c r="L22" t="n">
+        <v>480</v>
+      </c>
+      <c r="M22" t="n">
+        <v>485</v>
+      </c>
+      <c r="N22" t="n">
+        <v>505</v>
+      </c>
+      <c r="O22" t="n">
+        <v>545</v>
+      </c>
+      <c r="P22" t="n">
+        <v>480</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>618</v>
+      </c>
+      <c r="R22" t="n">
+        <v>490</v>
+      </c>
+      <c r="S22" t="n">
+        <v>474</v>
+      </c>
+      <c r="T22" t="n">
+        <v>480</v>
+      </c>
+      <c r="U22" t="n">
+        <v>619</v>
+      </c>
+      <c r="V22" t="n">
+        <v>550</v>
+      </c>
+      <c r="W22" t="n">
+        <v>599</v>
+      </c>
+      <c r="X22" t="n">
+        <v>495</v>
+      </c>
+      <c r="Y22" s="3" t="n">
+        <v>45754</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>850</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>555</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>543.5</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>500</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>545</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>507</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>509</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>745</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>473</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>735</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>474</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>488</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>570</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>555</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>488</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>535</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>547</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>568</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>547</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>645</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>634</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>496</v>
+      </c>
+      <c r="AV22" t="n">
         <v>485</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-14 02:42
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV25"/>
+  <dimension ref="A1:AV26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4083,7 +4083,7 @@
       <c r="X25" t="n">
         <v>490</v>
       </c>
-      <c r="Y25" s="3" t="n">
+      <c r="Y25" s="2" t="n">
         <v>45755</v>
       </c>
       <c r="Z25" t="n">
@@ -4154,6 +4154,152 @@
       </c>
       <c r="AV25" t="n">
         <v>470</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>550</v>
+      </c>
+      <c r="B26" t="n">
+        <v>462</v>
+      </c>
+      <c r="C26" t="n">
+        <v>435</v>
+      </c>
+      <c r="D26" t="n">
+        <v>535</v>
+      </c>
+      <c r="E26" t="n">
+        <v>506</v>
+      </c>
+      <c r="F26" t="n">
+        <v>514</v>
+      </c>
+      <c r="G26" t="n">
+        <v>461</v>
+      </c>
+      <c r="H26" t="n">
+        <v>555</v>
+      </c>
+      <c r="I26" t="n">
+        <v>500</v>
+      </c>
+      <c r="J26" t="n">
+        <v>435</v>
+      </c>
+      <c r="K26" t="n">
+        <v>573</v>
+      </c>
+      <c r="L26" t="n">
+        <v>465</v>
+      </c>
+      <c r="M26" t="n">
+        <v>460</v>
+      </c>
+      <c r="N26" t="n">
+        <v>491</v>
+      </c>
+      <c r="O26" t="n">
+        <v>550</v>
+      </c>
+      <c r="P26" t="n">
+        <v>465</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>620</v>
+      </c>
+      <c r="R26" t="n">
+        <v>485</v>
+      </c>
+      <c r="S26" t="n">
+        <v>461</v>
+      </c>
+      <c r="T26" t="n">
+        <v>465</v>
+      </c>
+      <c r="U26" t="n">
+        <v>621</v>
+      </c>
+      <c r="V26" t="n">
+        <v>535</v>
+      </c>
+      <c r="W26" t="n">
+        <v>590</v>
+      </c>
+      <c r="X26" t="n">
+        <v>475</v>
+      </c>
+      <c r="Y26" s="3" t="n">
+        <v>45756</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>848</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>557</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>535.5</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>494</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>543</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>507</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>509</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>733</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>455</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>723</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>461</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>472</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>545</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>536</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>472</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>519</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>539</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>567</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>550</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>640</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>639</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>487</v>
+      </c>
+      <c r="AV26" t="n">
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-14 03:00
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV28"/>
+  <dimension ref="A1:AV29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4521,7 +4521,7 @@
       <c r="X28" t="n">
         <v>490</v>
       </c>
-      <c r="Y28" s="3" t="n">
+      <c r="Y28" s="2" t="n">
         <v>45758</v>
       </c>
       <c r="Z28" t="n">
@@ -4592,6 +4592,152 @@
       </c>
       <c r="AV28" t="n">
         <v>475</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>565</v>
+      </c>
+      <c r="B29" t="n">
+        <v>474</v>
+      </c>
+      <c r="C29" t="n">
+        <v>450</v>
+      </c>
+      <c r="D29" t="n">
+        <v>522</v>
+      </c>
+      <c r="E29" t="n">
+        <v>515</v>
+      </c>
+      <c r="F29" t="n">
+        <v>520</v>
+      </c>
+      <c r="G29" t="n">
+        <v>474</v>
+      </c>
+      <c r="H29" t="n">
+        <v>570</v>
+      </c>
+      <c r="I29" t="n">
+        <v>490</v>
+      </c>
+      <c r="J29" t="n">
+        <v>450</v>
+      </c>
+      <c r="K29" t="n">
+        <v>571</v>
+      </c>
+      <c r="L29" t="n">
+        <v>480</v>
+      </c>
+      <c r="M29" t="n">
+        <v>485</v>
+      </c>
+      <c r="N29" t="n">
+        <v>505</v>
+      </c>
+      <c r="O29" t="n">
+        <v>545</v>
+      </c>
+      <c r="P29" t="n">
+        <v>480</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>618</v>
+      </c>
+      <c r="R29" t="n">
+        <v>490</v>
+      </c>
+      <c r="S29" t="n">
+        <v>474</v>
+      </c>
+      <c r="T29" t="n">
+        <v>480</v>
+      </c>
+      <c r="U29" t="n">
+        <v>619</v>
+      </c>
+      <c r="V29" t="n">
+        <v>550</v>
+      </c>
+      <c r="W29" t="n">
+        <v>599</v>
+      </c>
+      <c r="X29" t="n">
+        <v>495</v>
+      </c>
+      <c r="Y29" s="3" t="n">
+        <v>45754</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>850</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>555</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>543.5</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>500</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>545</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>507</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>509</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>745</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>473</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>735</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>474</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>488</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>570</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>555</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>488</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>535</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>547</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>568</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>547</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>645</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>634</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>496</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-14 03:01
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV29"/>
+  <dimension ref="A1:AV30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4667,7 +4667,7 @@
       <c r="X29" t="n">
         <v>495</v>
       </c>
-      <c r="Y29" s="3" t="n">
+      <c r="Y29" s="2" t="n">
         <v>45754</v>
       </c>
       <c r="Z29" t="n">
@@ -4738,6 +4738,152 @@
       </c>
       <c r="AV29" t="n">
         <v>485</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>567</v>
+      </c>
+      <c r="B30" t="n">
+        <v>478</v>
+      </c>
+      <c r="C30" t="n">
+        <v>442</v>
+      </c>
+      <c r="D30" t="n">
+        <v>549</v>
+      </c>
+      <c r="E30" t="n">
+        <v>494</v>
+      </c>
+      <c r="F30" t="n">
+        <v>532</v>
+      </c>
+      <c r="G30" t="n">
+        <v>475</v>
+      </c>
+      <c r="H30" t="n">
+        <v>569</v>
+      </c>
+      <c r="I30" t="n">
+        <v>512</v>
+      </c>
+      <c r="J30" t="n">
+        <v>442</v>
+      </c>
+      <c r="K30" t="n">
+        <v>571</v>
+      </c>
+      <c r="L30" t="n">
+        <v>483</v>
+      </c>
+      <c r="M30" t="n">
+        <v>447</v>
+      </c>
+      <c r="N30" t="n">
+        <v>505</v>
+      </c>
+      <c r="O30" t="n">
+        <v>555</v>
+      </c>
+      <c r="P30" t="n">
+        <v>483</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>619</v>
+      </c>
+      <c r="R30" t="n">
+        <v>495</v>
+      </c>
+      <c r="S30" t="n">
+        <v>475</v>
+      </c>
+      <c r="T30" t="n">
+        <v>480</v>
+      </c>
+      <c r="U30" t="n">
+        <v>620</v>
+      </c>
+      <c r="V30" t="n">
+        <v>530</v>
+      </c>
+      <c r="W30" t="n">
+        <v>589</v>
+      </c>
+      <c r="X30" t="n">
+        <v>475</v>
+      </c>
+      <c r="Y30" s="3" t="n">
+        <v>45757</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>846</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>555</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>519.5</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>512</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>538</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>500</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>502</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>750</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>459</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>740</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>475</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>486</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>550</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>535</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>487</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>536</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>523</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>563</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>545</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>620</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>632</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>489</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-14 03:39
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV30"/>
+  <dimension ref="A1:AV31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4813,7 +4813,7 @@
       <c r="X30" t="n">
         <v>475</v>
       </c>
-      <c r="Y30" s="3" t="n">
+      <c r="Y30" s="2" t="n">
         <v>45757</v>
       </c>
       <c r="Z30" t="n">
@@ -4884,6 +4884,152 @@
       </c>
       <c r="AV30" t="n">
         <v>470</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>565</v>
+      </c>
+      <c r="B31" t="n">
+        <v>479</v>
+      </c>
+      <c r="C31" t="n">
+        <v>450</v>
+      </c>
+      <c r="D31" t="n">
+        <v>548</v>
+      </c>
+      <c r="E31" t="n">
+        <v>498</v>
+      </c>
+      <c r="F31" t="n">
+        <v>532</v>
+      </c>
+      <c r="G31" t="n">
+        <v>474</v>
+      </c>
+      <c r="H31" t="n">
+        <v>567</v>
+      </c>
+      <c r="I31" t="n">
+        <v>495</v>
+      </c>
+      <c r="J31" t="n">
+        <v>450</v>
+      </c>
+      <c r="K31" t="n">
+        <v>572</v>
+      </c>
+      <c r="L31" t="n">
+        <v>483</v>
+      </c>
+      <c r="M31" t="n">
+        <v>462</v>
+      </c>
+      <c r="N31" t="n">
+        <v>505</v>
+      </c>
+      <c r="O31" t="n">
+        <v>557</v>
+      </c>
+      <c r="P31" t="n">
+        <v>483</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>618</v>
+      </c>
+      <c r="R31" t="n">
+        <v>497</v>
+      </c>
+      <c r="S31" t="n">
+        <v>474</v>
+      </c>
+      <c r="T31" t="n">
+        <v>485</v>
+      </c>
+      <c r="U31" t="n">
+        <v>619</v>
+      </c>
+      <c r="V31" t="n">
+        <v>540</v>
+      </c>
+      <c r="W31" t="n">
+        <v>594</v>
+      </c>
+      <c r="X31" t="n">
+        <v>490</v>
+      </c>
+      <c r="Y31" s="3" t="n">
+        <v>45758</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>818</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>556</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>525.5</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>512</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>542</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>504</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>506</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>730</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>467</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>720</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>474</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>484</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>550</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>540</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>485</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>540</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>529</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>565</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>546</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>635</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>637</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>493</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-14 03:55
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV31"/>
+  <dimension ref="A1:AV32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4959,7 +4959,7 @@
       <c r="X31" t="n">
         <v>490</v>
       </c>
-      <c r="Y31" s="3" t="n">
+      <c r="Y31" s="2" t="n">
         <v>45758</v>
       </c>
       <c r="Z31" t="n">
@@ -5029,6 +5029,152 @@
         <v>493</v>
       </c>
       <c r="AV31" t="n">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>565</v>
+      </c>
+      <c r="B32" t="n">
+        <v>479</v>
+      </c>
+      <c r="C32" t="n">
+        <v>450</v>
+      </c>
+      <c r="D32" t="n">
+        <v>548</v>
+      </c>
+      <c r="E32" t="n">
+        <v>498</v>
+      </c>
+      <c r="F32" t="n">
+        <v>532</v>
+      </c>
+      <c r="G32" t="n">
+        <v>474</v>
+      </c>
+      <c r="H32" t="n">
+        <v>567</v>
+      </c>
+      <c r="I32" t="n">
+        <v>495</v>
+      </c>
+      <c r="J32" t="n">
+        <v>450</v>
+      </c>
+      <c r="K32" t="n">
+        <v>572</v>
+      </c>
+      <c r="L32" t="n">
+        <v>483</v>
+      </c>
+      <c r="M32" t="n">
+        <v>462</v>
+      </c>
+      <c r="N32" t="n">
+        <v>505</v>
+      </c>
+      <c r="O32" t="n">
+        <v>557</v>
+      </c>
+      <c r="P32" t="n">
+        <v>483</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>618</v>
+      </c>
+      <c r="R32" t="n">
+        <v>497</v>
+      </c>
+      <c r="S32" t="n">
+        <v>474</v>
+      </c>
+      <c r="T32" t="n">
+        <v>485</v>
+      </c>
+      <c r="U32" t="n">
+        <v>619</v>
+      </c>
+      <c r="V32" t="n">
+        <v>540</v>
+      </c>
+      <c r="W32" t="n">
+        <v>594</v>
+      </c>
+      <c r="X32" t="n">
+        <v>490</v>
+      </c>
+      <c r="Y32" s="3" t="n">
+        <v>45758</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>818</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>556</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>525.5</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>512</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>542</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>504</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>506</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>730</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>467</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>720</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>474</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>484</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>550</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>540</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>485</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>540</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>529</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>565</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>546</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>635</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>637</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>493</v>
+      </c>
+      <c r="AV32" t="n">
         <v>475</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-18 06:01
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU25"/>
+  <dimension ref="A1:AU26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4076,6 +4076,149 @@
         <v>638</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B26" t="n">
+        <v>485</v>
+      </c>
+      <c r="C26" t="n">
+        <v>480</v>
+      </c>
+      <c r="D26" t="n">
+        <v>520</v>
+      </c>
+      <c r="E26" t="n">
+        <v>540</v>
+      </c>
+      <c r="F26" t="n">
+        <v>535</v>
+      </c>
+      <c r="G26" t="n">
+        <v>540</v>
+      </c>
+      <c r="H26" t="n">
+        <v>505</v>
+      </c>
+      <c r="I26" t="n">
+        <v>486</v>
+      </c>
+      <c r="J26" t="n">
+        <v>485</v>
+      </c>
+      <c r="K26" t="n">
+        <v>711</v>
+      </c>
+      <c r="L26" t="n">
+        <v>721</v>
+      </c>
+      <c r="M26" t="n">
+        <v>480</v>
+      </c>
+      <c r="N26" t="n">
+        <v>480</v>
+      </c>
+      <c r="O26" t="n">
+        <v>558</v>
+      </c>
+      <c r="P26" t="n">
+        <v>560</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>483</v>
+      </c>
+      <c r="R26" t="n">
+        <v>625</v>
+      </c>
+      <c r="S26" t="n">
+        <v>483</v>
+      </c>
+      <c r="T26" t="n">
+        <v>490</v>
+      </c>
+      <c r="U26" t="n">
+        <v>535</v>
+      </c>
+      <c r="V26" t="n">
+        <v>445</v>
+      </c>
+      <c r="W26" t="n">
+        <v>445</v>
+      </c>
+      <c r="X26" t="n">
+        <v>477</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>478</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>570</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>490</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>490</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>485</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>560</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>470</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>492</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>548</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>494</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>494</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>527</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>523.5</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>546</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>544</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>502</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>813</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>600</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>612</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>611</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>567</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>594</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>636</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-18 06:02
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU26"/>
+  <dimension ref="A1:AU27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4219,6 +4219,149 @@
         <v>636</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45763</v>
+      </c>
+      <c r="B27" t="n">
+        <v>485</v>
+      </c>
+      <c r="C27" t="n">
+        <v>481</v>
+      </c>
+      <c r="D27" t="n">
+        <v>518</v>
+      </c>
+      <c r="E27" t="n">
+        <v>538</v>
+      </c>
+      <c r="F27" t="n">
+        <v>550.25</v>
+      </c>
+      <c r="G27" t="n">
+        <v>540</v>
+      </c>
+      <c r="H27" t="n">
+        <v>504</v>
+      </c>
+      <c r="I27" t="n">
+        <v>488</v>
+      </c>
+      <c r="J27" t="n">
+        <v>487</v>
+      </c>
+      <c r="K27" t="n">
+        <v>709</v>
+      </c>
+      <c r="L27" t="n">
+        <v>719</v>
+      </c>
+      <c r="M27" t="n">
+        <v>481</v>
+      </c>
+      <c r="N27" t="n">
+        <v>481</v>
+      </c>
+      <c r="O27" t="n">
+        <v>557</v>
+      </c>
+      <c r="P27" t="n">
+        <v>559</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>486</v>
+      </c>
+      <c r="R27" t="n">
+        <v>625</v>
+      </c>
+      <c r="S27" t="n">
+        <v>486</v>
+      </c>
+      <c r="T27" t="n">
+        <v>490</v>
+      </c>
+      <c r="U27" t="n">
+        <v>540</v>
+      </c>
+      <c r="V27" t="n">
+        <v>450</v>
+      </c>
+      <c r="W27" t="n">
+        <v>450</v>
+      </c>
+      <c r="X27" t="n">
+        <v>477</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>476</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>565</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>495</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>490</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>484</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>580</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>471</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>497</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>547</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>495</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>499</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>530</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>526.5</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>548</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>545</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>500</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>814</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>598</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>613</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>612</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>569</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>593</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>640</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-21 02:42
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU27"/>
+  <dimension ref="A1:AU28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4362,6 +4362,149 @@
         <v>640</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45764</v>
+      </c>
+      <c r="B28" t="n">
+        <v>489</v>
+      </c>
+      <c r="C28" t="n">
+        <v>484</v>
+      </c>
+      <c r="D28" t="n">
+        <v>524</v>
+      </c>
+      <c r="E28" t="n">
+        <v>544</v>
+      </c>
+      <c r="F28" t="n">
+        <v>535</v>
+      </c>
+      <c r="G28" t="n">
+        <v>535</v>
+      </c>
+      <c r="H28" t="n">
+        <v>510</v>
+      </c>
+      <c r="I28" t="n">
+        <v>493</v>
+      </c>
+      <c r="J28" t="n">
+        <v>492</v>
+      </c>
+      <c r="K28" t="n">
+        <v>718</v>
+      </c>
+      <c r="L28" t="n">
+        <v>728</v>
+      </c>
+      <c r="M28" t="n">
+        <v>484</v>
+      </c>
+      <c r="N28" t="n">
+        <v>484</v>
+      </c>
+      <c r="O28" t="n">
+        <v>558</v>
+      </c>
+      <c r="P28" t="n">
+        <v>560</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>480</v>
+      </c>
+      <c r="R28" t="n">
+        <v>635</v>
+      </c>
+      <c r="S28" t="n">
+        <v>480</v>
+      </c>
+      <c r="T28" t="n">
+        <v>485</v>
+      </c>
+      <c r="U28" t="n">
+        <v>537</v>
+      </c>
+      <c r="V28" t="n">
+        <v>450</v>
+      </c>
+      <c r="W28" t="n">
+        <v>450</v>
+      </c>
+      <c r="X28" t="n">
+        <v>482</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>475</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>570</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>490</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>490</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>483</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>580</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>480</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>501</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>549</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>496</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>503</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>540</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>536.5</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>551</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>548</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>503</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>779</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>607</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>608</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>607</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>571</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>595</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>647</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-04-21 09:22
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -610,77 +610,77 @@
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
+          <t>St. Petersburg</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
           <t>Colombo</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Los Angeles</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Lome</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Houston</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Lisbon</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Japan</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Melbourne</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Cartagena</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>West Japan</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Sydney</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Vancouver</t>
-        </is>
-      </c>
-      <c r="AW1" s="1" t="inlineStr">
-        <is>
-          <t>St. Petersburg</t>
         </is>
       </c>
     </row>
@@ -745,9 +745,7 @@
       <c r="T2" t="n">
         <v>484</v>
       </c>
-      <c r="U2" t="n">
-        <v>520</v>
-      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="n">
         <v>496</v>
       </c>
@@ -787,71 +785,71 @@
       <c r="AH2" t="n">
         <v>537</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="n">
         <v>560</v>
       </c>
-      <c r="AJ2" s="2" t="n">
+      <c r="AK2" s="2" t="n">
         <v>45764</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AL2" t="n">
         <v>549</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AM2" t="n">
         <v>580</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AN2" t="n">
         <v>480</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AO2" t="n">
         <v>483</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AP2" t="n">
         <v>489</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AQ2" t="n">
         <v>524</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AR2" t="n">
         <v>728</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AS2" t="n">
         <v>548</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AT2" t="n">
         <v>595</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AU2" t="n">
         <v>544</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AV2" t="n">
         <v>718</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AW2" t="n">
         <v>536.5</v>
       </c>
-      <c r="AW2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>490</v>
       </c>
       <c r="B3" t="n">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C3" t="n">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="D3" t="n">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="E3" t="n">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="F3" t="n">
+        <v>495</v>
+      </c>
+      <c r="G3" t="n">
         <v>490</v>
-      </c>
-      <c r="G3" t="n">
-        <v>485</v>
       </c>
       <c r="H3" t="n">
         <v>450</v>
@@ -860,121 +858,121 @@
         <v>450</v>
       </c>
       <c r="J3" t="n">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K3" t="n">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="L3" t="n">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="M3" t="n">
-        <v>779</v>
+        <v>814</v>
       </c>
       <c r="N3" t="n">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="O3" t="n">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="P3" t="n">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="Q3" t="n">
-        <v>535</v>
+        <v>550.25</v>
       </c>
       <c r="R3" t="n">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="S3" t="n">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="T3" t="n">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="n">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="W3" t="n">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="X3" t="n">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="Y3" t="n">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="Z3" t="n">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="AA3" t="n">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="AB3" t="n">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="AC3" t="n">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="AD3" t="n">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="AE3" t="n">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="AF3" t="n">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="AG3" t="n">
+        <v>481</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>540</v>
+      </c>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="n">
+        <v>559</v>
+      </c>
+      <c r="AK3" s="2" t="n">
+        <v>45763</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>547</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>580</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>471</v>
+      </c>
+      <c r="AO3" t="n">
         <v>484</v>
       </c>
-      <c r="AH3" t="n">
-        <v>537</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>560</v>
-      </c>
-      <c r="AJ3" s="2" t="n">
-        <v>45764</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>549</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>580</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>480</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>483</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>489</v>
-      </c>
       <c r="AP3" t="n">
-        <v>524</v>
+        <v>485</v>
       </c>
       <c r="AQ3" t="n">
-        <v>728</v>
+        <v>518</v>
       </c>
       <c r="AR3" t="n">
-        <v>548</v>
+        <v>719</v>
       </c>
       <c r="AS3" t="n">
-        <v>595</v>
+        <v>545</v>
       </c>
       <c r="AT3" t="n">
-        <v>544</v>
+        <v>593</v>
       </c>
       <c r="AU3" t="n">
-        <v>718</v>
+        <v>538</v>
       </c>
       <c r="AV3" t="n">
-        <v>536.5</v>
-      </c>
-      <c r="AW3" t="inlineStr"/>
+        <v>709</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>526.5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1037,7 +1035,9 @@
       <c r="T4" t="n">
         <v>481</v>
       </c>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="n">
+        <v>526</v>
+      </c>
       <c r="V4" t="n">
         <v>495</v>
       </c>
@@ -1077,49 +1077,49 @@
       <c r="AH4" t="n">
         <v>540</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="n">
         <v>559</v>
       </c>
-      <c r="AJ4" s="2" t="n">
+      <c r="AK4" s="2" t="n">
         <v>45763</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AL4" t="n">
         <v>547</v>
       </c>
-      <c r="AL4" t="n">
+      <c r="AM4" t="n">
         <v>580</v>
       </c>
-      <c r="AM4" t="n">
+      <c r="AN4" t="n">
         <v>471</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AO4" t="n">
         <v>484</v>
       </c>
-      <c r="AO4" t="n">
+      <c r="AP4" t="n">
         <v>485</v>
       </c>
-      <c r="AP4" t="n">
+      <c r="AQ4" t="n">
         <v>518</v>
       </c>
-      <c r="AQ4" t="n">
+      <c r="AR4" t="n">
         <v>719</v>
       </c>
-      <c r="AR4" t="n">
+      <c r="AS4" t="n">
         <v>545</v>
       </c>
-      <c r="AS4" t="n">
+      <c r="AT4" t="n">
         <v>593</v>
       </c>
-      <c r="AT4" t="n">
+      <c r="AU4" t="n">
         <v>538</v>
       </c>
-      <c r="AU4" t="n">
+      <c r="AV4" t="n">
         <v>709</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="AW4" t="n">
         <v>526.5</v>
       </c>
-      <c r="AW4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1222,49 +1222,49 @@
       <c r="AH5" t="n">
         <v>535</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="n">
         <v>560</v>
       </c>
-      <c r="AJ5" s="2" t="n">
+      <c r="AK5" s="2" t="n">
         <v>45762</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AL5" t="n">
         <v>548</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="AM5" t="n">
         <v>560</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AN5" t="n">
         <v>470</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>485</v>
       </c>
       <c r="AO5" t="n">
         <v>485</v>
       </c>
       <c r="AP5" t="n">
+        <v>485</v>
+      </c>
+      <c r="AQ5" t="n">
         <v>520</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AR5" t="n">
         <v>721</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AS5" t="n">
         <v>544</v>
       </c>
-      <c r="AS5" t="n">
+      <c r="AT5" t="n">
         <v>594</v>
       </c>
-      <c r="AT5" t="n">
+      <c r="AU5" t="n">
         <v>540</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="AV5" t="n">
         <v>711</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="AW5" t="n">
         <v>523.5</v>
       </c>
-      <c r="AW5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1367,49 +1367,49 @@
       <c r="AH6" t="n">
         <v>540</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="n">
         <v>567</v>
       </c>
-      <c r="AJ6" s="2" t="n">
+      <c r="AK6" s="2" t="n">
         <v>45761</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AL6" t="n">
         <v>543</v>
       </c>
-      <c r="AL6" t="n">
+      <c r="AM6" t="n">
         <v>560</v>
       </c>
-      <c r="AM6" t="n">
+      <c r="AN6" t="n">
         <v>465</v>
       </c>
-      <c r="AN6" t="n">
+      <c r="AO6" t="n">
         <v>482</v>
       </c>
-      <c r="AO6" t="n">
+      <c r="AP6" t="n">
         <v>488</v>
       </c>
-      <c r="AP6" t="n">
+      <c r="AQ6" t="n">
         <v>521</v>
       </c>
-      <c r="AQ6" t="n">
+      <c r="AR6" t="n">
         <v>723</v>
       </c>
-      <c r="AR6" t="n">
+      <c r="AS6" t="n">
         <v>549</v>
       </c>
-      <c r="AS6" t="n">
+      <c r="AT6" t="n">
         <v>587</v>
       </c>
-      <c r="AT6" t="n">
+      <c r="AU6" t="n">
         <v>541</v>
       </c>
-      <c r="AU6" t="n">
+      <c r="AV6" t="n">
         <v>713</v>
       </c>
-      <c r="AV6" t="n">
+      <c r="AW6" t="n">
         <v>524.5</v>
       </c>
-      <c r="AW6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1512,49 +1512,49 @@
       <c r="AH7" t="n">
         <v>540</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="n">
         <v>567</v>
       </c>
-      <c r="AJ7" s="2" t="n">
+      <c r="AK7" s="2" t="n">
         <v>45758</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AL7" t="n">
         <v>556</v>
       </c>
-      <c r="AL7" t="n">
+      <c r="AM7" t="n">
         <v>550</v>
       </c>
-      <c r="AM7" t="n">
+      <c r="AN7" t="n">
         <v>467</v>
       </c>
-      <c r="AN7" t="n">
+      <c r="AO7" t="n">
         <v>495</v>
       </c>
-      <c r="AO7" t="n">
+      <c r="AP7" t="n">
         <v>479</v>
       </c>
-      <c r="AP7" t="n">
+      <c r="AQ7" t="n">
         <v>512</v>
       </c>
-      <c r="AQ7" t="n">
+      <c r="AR7" t="n">
         <v>730</v>
       </c>
-      <c r="AR7" t="n">
+      <c r="AS7" t="n">
         <v>546</v>
       </c>
-      <c r="AS7" t="n">
+      <c r="AT7" t="n">
         <v>572</v>
       </c>
-      <c r="AT7" t="n">
+      <c r="AU7" t="n">
         <v>532</v>
       </c>
-      <c r="AU7" t="n">
+      <c r="AV7" t="n">
         <v>720</v>
       </c>
-      <c r="AV7" t="n">
+      <c r="AW7" t="n">
         <v>525.5</v>
       </c>
-      <c r="AW7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1657,49 +1657,49 @@
       <c r="AH8" t="n">
         <v>535</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="n">
         <v>569</v>
       </c>
-      <c r="AJ8" s="2" t="n">
+      <c r="AK8" s="2" t="n">
         <v>45757</v>
       </c>
-      <c r="AK8" t="n">
+      <c r="AL8" t="n">
         <v>555</v>
       </c>
-      <c r="AL8" t="n">
+      <c r="AM8" t="n">
         <v>550</v>
       </c>
-      <c r="AM8" t="n">
+      <c r="AN8" t="n">
         <v>459</v>
       </c>
-      <c r="AN8" t="n">
+      <c r="AO8" t="n">
         <v>512</v>
       </c>
-      <c r="AO8" t="n">
+      <c r="AP8" t="n">
         <v>478</v>
       </c>
-      <c r="AP8" t="n">
+      <c r="AQ8" t="n">
         <v>512</v>
       </c>
-      <c r="AQ8" t="n">
+      <c r="AR8" t="n">
         <v>750</v>
       </c>
-      <c r="AR8" t="n">
+      <c r="AS8" t="n">
         <v>545</v>
       </c>
-      <c r="AS8" t="n">
+      <c r="AT8" t="n">
         <v>571</v>
       </c>
-      <c r="AT8" t="n">
+      <c r="AU8" t="n">
         <v>532</v>
       </c>
-      <c r="AU8" t="n">
+      <c r="AV8" t="n">
         <v>740</v>
       </c>
-      <c r="AV8" t="n">
+      <c r="AW8" t="n">
         <v>519.5</v>
       </c>
-      <c r="AW8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1802,49 +1802,49 @@
       <c r="AH9" t="n">
         <v>536</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="n">
         <v>555</v>
       </c>
-      <c r="AJ9" s="2" t="n">
+      <c r="AK9" s="2" t="n">
         <v>45756</v>
       </c>
-      <c r="AK9" t="n">
+      <c r="AL9" t="n">
         <v>557</v>
       </c>
-      <c r="AL9" t="n">
+      <c r="AM9" t="n">
         <v>545</v>
       </c>
-      <c r="AM9" t="n">
+      <c r="AN9" t="n">
         <v>455</v>
       </c>
-      <c r="AN9" t="n">
+      <c r="AO9" t="n">
         <v>500</v>
       </c>
-      <c r="AO9" t="n">
+      <c r="AP9" t="n">
         <v>462</v>
       </c>
-      <c r="AP9" t="n">
+      <c r="AQ9" t="n">
         <v>494</v>
       </c>
-      <c r="AQ9" t="n">
+      <c r="AR9" t="n">
         <v>733</v>
       </c>
-      <c r="AR9" t="n">
+      <c r="AS9" t="n">
         <v>550</v>
       </c>
-      <c r="AS9" t="n">
+      <c r="AT9" t="n">
         <v>573</v>
       </c>
-      <c r="AT9" t="n">
+      <c r="AU9" t="n">
         <v>514</v>
       </c>
-      <c r="AU9" t="n">
+      <c r="AV9" t="n">
         <v>723</v>
       </c>
-      <c r="AV9" t="n">
+      <c r="AW9" t="n">
         <v>535.5</v>
       </c>
-      <c r="AW9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1947,49 +1947,49 @@
       <c r="AH10" t="n">
         <v>540</v>
       </c>
-      <c r="AI10" t="n">
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="n">
         <v>565</v>
       </c>
-      <c r="AJ10" s="2" t="n">
+      <c r="AK10" s="2" t="n">
         <v>45755</v>
       </c>
-      <c r="AK10" t="n">
+      <c r="AL10" t="n">
         <v>554</v>
       </c>
-      <c r="AL10" t="n">
+      <c r="AM10" t="n">
         <v>560</v>
       </c>
-      <c r="AM10" t="n">
+      <c r="AN10" t="n">
         <v>464</v>
       </c>
-      <c r="AN10" t="n">
+      <c r="AO10" t="n">
         <v>500</v>
       </c>
-      <c r="AO10" t="n">
+      <c r="AP10" t="n">
         <v>477</v>
       </c>
-      <c r="AP10" t="n">
+      <c r="AQ10" t="n">
         <v>504</v>
       </c>
-      <c r="AQ10" t="n">
+      <c r="AR10" t="n">
         <v>749</v>
       </c>
-      <c r="AR10" t="n">
+      <c r="AS10" t="n">
         <v>546</v>
       </c>
-      <c r="AS10" t="n">
+      <c r="AT10" t="n">
         <v>570</v>
       </c>
-      <c r="AT10" t="n">
+      <c r="AU10" t="n">
         <v>524</v>
       </c>
-      <c r="AU10" t="n">
+      <c r="AV10" t="n">
         <v>739</v>
       </c>
-      <c r="AV10" t="n">
+      <c r="AW10" t="n">
         <v>549.5</v>
       </c>
-      <c r="AW10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -2092,49 +2092,49 @@
       <c r="AH11" t="n">
         <v>555</v>
       </c>
-      <c r="AI11" t="n">
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="n">
         <v>570</v>
       </c>
-      <c r="AJ11" s="2" t="n">
+      <c r="AK11" s="2" t="n">
         <v>45754</v>
       </c>
-      <c r="AK11" t="n">
+      <c r="AL11" t="n">
         <v>555</v>
       </c>
-      <c r="AL11" t="n">
+      <c r="AM11" t="n">
         <v>570</v>
       </c>
-      <c r="AM11" t="n">
+      <c r="AN11" t="n">
         <v>473</v>
       </c>
-      <c r="AN11" t="n">
+      <c r="AO11" t="n">
         <v>490</v>
       </c>
-      <c r="AO11" t="n">
+      <c r="AP11" t="n">
         <v>474</v>
       </c>
-      <c r="AP11" t="n">
+      <c r="AQ11" t="n">
         <v>500</v>
       </c>
-      <c r="AQ11" t="n">
+      <c r="AR11" t="n">
         <v>745</v>
       </c>
-      <c r="AR11" t="n">
+      <c r="AS11" t="n">
         <v>547</v>
       </c>
-      <c r="AS11" t="n">
+      <c r="AT11" t="n">
         <v>571</v>
       </c>
-      <c r="AT11" t="n">
+      <c r="AU11" t="n">
         <v>520</v>
       </c>
-      <c r="AU11" t="n">
+      <c r="AV11" t="n">
         <v>735</v>
       </c>
-      <c r="AV11" t="n">
+      <c r="AW11" t="n">
         <v>543.5</v>
       </c>
-      <c r="AW11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -2237,49 +2237,49 @@
       <c r="AH12" t="n">
         <v>570</v>
       </c>
-      <c r="AI12" t="n">
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="n">
         <v>585</v>
       </c>
-      <c r="AJ12" s="2" t="n">
+      <c r="AK12" s="2" t="n">
         <v>45751</v>
       </c>
-      <c r="AK12" t="n">
+      <c r="AL12" t="n">
         <v>570</v>
       </c>
-      <c r="AL12" t="n">
+      <c r="AM12" t="n">
         <v>590</v>
       </c>
-      <c r="AM12" t="n">
+      <c r="AN12" t="n">
         <v>490</v>
       </c>
-      <c r="AN12" t="n">
+      <c r="AO12" t="n">
         <v>515</v>
       </c>
-      <c r="AO12" t="n">
+      <c r="AP12" t="n">
         <v>498</v>
       </c>
-      <c r="AP12" t="n">
+      <c r="AQ12" t="n">
         <v>525</v>
       </c>
-      <c r="AQ12" t="n">
+      <c r="AR12" t="n">
         <v>770</v>
       </c>
-      <c r="AR12" t="n">
+      <c r="AS12" t="n">
         <v>555</v>
       </c>
-      <c r="AS12" t="n">
+      <c r="AT12" t="n">
         <v>586</v>
       </c>
-      <c r="AT12" t="n">
+      <c r="AU12" t="n">
         <v>544</v>
       </c>
-      <c r="AU12" t="n">
+      <c r="AV12" t="n">
         <v>760</v>
       </c>
-      <c r="AV12" t="n">
+      <c r="AW12" t="n">
         <v>555.5</v>
       </c>
-      <c r="AW12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -2382,49 +2382,49 @@
       <c r="AH13" t="n">
         <v>592</v>
       </c>
-      <c r="AI13" t="n">
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="n">
         <v>595</v>
       </c>
-      <c r="AJ13" s="2" t="n">
+      <c r="AK13" s="2" t="n">
         <v>45750</v>
       </c>
-      <c r="AK13" t="n">
+      <c r="AL13" t="n">
         <v>621</v>
       </c>
-      <c r="AL13" t="n">
+      <c r="AM13" t="n">
         <v>615</v>
       </c>
-      <c r="AM13" t="n">
+      <c r="AN13" t="n">
         <v>511</v>
       </c>
-      <c r="AN13" t="n">
+      <c r="AO13" t="n">
         <v>535</v>
       </c>
-      <c r="AO13" t="n">
+      <c r="AP13" t="n">
         <v>524</v>
       </c>
-      <c r="AP13" t="n">
+      <c r="AQ13" t="n">
         <v>555</v>
       </c>
-      <c r="AQ13" t="n">
+      <c r="AR13" t="n">
         <v>776</v>
       </c>
-      <c r="AR13" t="n">
+      <c r="AS13" t="n">
         <v>570</v>
       </c>
-      <c r="AS13" t="n">
+      <c r="AT13" t="n">
         <v>637</v>
       </c>
-      <c r="AT13" t="n">
+      <c r="AU13" t="n">
         <v>574</v>
       </c>
-      <c r="AU13" t="n">
+      <c r="AV13" t="n">
         <v>766</v>
       </c>
-      <c r="AV13" t="n">
+      <c r="AW13" t="n">
         <v>612.5</v>
       </c>
-      <c r="AW13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -2527,49 +2527,49 @@
       <c r="AH14" t="n">
         <v>595</v>
       </c>
-      <c r="AI14" t="n">
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="n">
         <v>600</v>
       </c>
-      <c r="AJ14" s="2" t="n">
+      <c r="AK14" s="2" t="n">
         <v>45749</v>
       </c>
-      <c r="AK14" t="n">
+      <c r="AL14" t="n">
         <v>629</v>
       </c>
-      <c r="AL14" t="n">
+      <c r="AM14" t="n">
         <v>625</v>
       </c>
-      <c r="AM14" t="n">
+      <c r="AN14" t="n">
         <v>537</v>
       </c>
-      <c r="AN14" t="n">
+      <c r="AO14" t="n">
         <v>542</v>
       </c>
-      <c r="AO14" t="n">
+      <c r="AP14" t="n">
         <v>535</v>
       </c>
-      <c r="AP14" t="n">
+      <c r="AQ14" t="n">
         <v>564</v>
       </c>
-      <c r="AQ14" t="n">
+      <c r="AR14" t="n">
         <v>788</v>
       </c>
-      <c r="AR14" t="n">
+      <c r="AS14" t="n">
         <v>584</v>
       </c>
-      <c r="AS14" t="n">
+      <c r="AT14" t="n">
         <v>645</v>
       </c>
-      <c r="AT14" t="n">
+      <c r="AU14" t="n">
         <v>584</v>
       </c>
-      <c r="AU14" t="n">
+      <c r="AV14" t="n">
         <v>778</v>
       </c>
-      <c r="AV14" t="n">
+      <c r="AW14" t="n">
         <v>619.5</v>
       </c>
-      <c r="AW14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2672,49 +2672,49 @@
       <c r="AH15" t="n">
         <v>595</v>
       </c>
-      <c r="AI15" t="n">
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="n">
         <v>595</v>
       </c>
-      <c r="AJ15" s="2" t="n">
+      <c r="AK15" s="2" t="n">
         <v>45748</v>
       </c>
-      <c r="AK15" t="n">
+      <c r="AL15" t="n">
         <v>628</v>
       </c>
-      <c r="AL15" t="n">
+      <c r="AM15" t="n">
         <v>630</v>
-      </c>
-      <c r="AM15" t="n">
-        <v>540</v>
       </c>
       <c r="AN15" t="n">
         <v>540</v>
       </c>
       <c r="AO15" t="n">
+        <v>540</v>
+      </c>
+      <c r="AP15" t="n">
         <v>533</v>
       </c>
-      <c r="AP15" t="n">
+      <c r="AQ15" t="n">
         <v>564</v>
       </c>
-      <c r="AQ15" t="n">
+      <c r="AR15" t="n">
         <v>785</v>
       </c>
-      <c r="AR15" t="n">
+      <c r="AS15" t="n">
         <v>581</v>
       </c>
-      <c r="AS15" t="n">
+      <c r="AT15" t="n">
         <v>644</v>
       </c>
-      <c r="AT15" t="n">
+      <c r="AU15" t="n">
         <v>584</v>
       </c>
-      <c r="AU15" t="n">
+      <c r="AV15" t="n">
         <v>775</v>
       </c>
-      <c r="AV15" t="n">
+      <c r="AW15" t="n">
         <v>617.5</v>
       </c>
-      <c r="AW15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2800,36 +2800,36 @@
         <v>590</v>
       </c>
       <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" s="2" t="n">
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" s="2" t="n">
         <v>45747</v>
       </c>
-      <c r="AK16" t="n">
+      <c r="AL16" t="n">
         <v>624</v>
       </c>
-      <c r="AL16" t="n">
+      <c r="AM16" t="n">
         <v>630</v>
       </c>
-      <c r="AM16" t="n">
+      <c r="AN16" t="n">
         <v>543</v>
       </c>
-      <c r="AN16" t="n">
+      <c r="AO16" t="n">
         <v>537</v>
       </c>
-      <c r="AO16" t="inlineStr"/>
       <c r="AP16" t="inlineStr"/>
       <c r="AQ16" t="inlineStr"/>
-      <c r="AR16" t="n">
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="n">
         <v>580</v>
       </c>
-      <c r="AS16" t="n">
+      <c r="AT16" t="n">
         <v>640</v>
       </c>
-      <c r="AT16" t="inlineStr"/>
       <c r="AU16" t="inlineStr"/>
-      <c r="AV16" t="n">
+      <c r="AV16" t="inlineStr"/>
+      <c r="AW16" t="n">
         <v>609.5</v>
       </c>
-      <c r="AW16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2932,49 +2932,49 @@
       <c r="AH17" t="n">
         <v>590</v>
       </c>
-      <c r="AI17" t="n">
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="n">
         <v>583</v>
       </c>
-      <c r="AJ17" s="2" t="n">
+      <c r="AK17" s="2" t="n">
         <v>45744</v>
       </c>
-      <c r="AK17" t="n">
+      <c r="AL17" t="n">
         <v>619</v>
       </c>
-      <c r="AL17" t="n">
+      <c r="AM17" t="n">
         <v>627</v>
       </c>
-      <c r="AM17" t="n">
+      <c r="AN17" t="n">
         <v>546</v>
       </c>
-      <c r="AN17" t="n">
+      <c r="AO17" t="n">
         <v>535</v>
       </c>
-      <c r="AO17" t="n">
+      <c r="AP17" t="n">
         <v>522</v>
       </c>
-      <c r="AP17" t="n">
+      <c r="AQ17" t="n">
         <v>555</v>
       </c>
-      <c r="AQ17" t="n">
+      <c r="AR17" t="n">
         <v>776</v>
       </c>
-      <c r="AR17" t="n">
+      <c r="AS17" t="n">
         <v>575</v>
       </c>
-      <c r="AS17" t="n">
+      <c r="AT17" t="n">
         <v>655</v>
       </c>
-      <c r="AT17" t="n">
+      <c r="AU17" t="n">
         <v>575</v>
       </c>
-      <c r="AU17" t="n">
+      <c r="AV17" t="n">
         <v>766</v>
       </c>
-      <c r="AV17" t="n">
+      <c r="AW17" t="n">
         <v>607.5</v>
       </c>
-      <c r="AW17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -3077,49 +3077,49 @@
       <c r="AH18" t="n">
         <v>592</v>
       </c>
-      <c r="AI18" t="n">
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="n">
         <v>580</v>
       </c>
-      <c r="AJ18" s="2" t="n">
+      <c r="AK18" s="2" t="n">
         <v>45743</v>
-      </c>
-      <c r="AK18" t="n">
-        <v>629</v>
       </c>
       <c r="AL18" t="n">
         <v>629</v>
       </c>
       <c r="AM18" t="n">
+        <v>629</v>
+      </c>
+      <c r="AN18" t="n">
         <v>536</v>
       </c>
-      <c r="AN18" t="n">
+      <c r="AO18" t="n">
         <v>535</v>
       </c>
-      <c r="AO18" t="n">
+      <c r="AP18" t="n">
         <v>521</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AQ18" t="n">
         <v>552</v>
       </c>
-      <c r="AQ18" t="n">
+      <c r="AR18" t="n">
         <v>772</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AS18" t="n">
         <v>576</v>
       </c>
-      <c r="AS18" t="n">
+      <c r="AT18" t="n">
         <v>665</v>
       </c>
-      <c r="AT18" t="n">
+      <c r="AU18" t="n">
         <v>572</v>
       </c>
-      <c r="AU18" t="n">
+      <c r="AV18" t="n">
         <v>762</v>
       </c>
-      <c r="AV18" t="n">
+      <c r="AW18" t="n">
         <v>606.5</v>
       </c>
-      <c r="AW18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -3222,49 +3222,49 @@
       <c r="AH19" t="n">
         <v>590</v>
       </c>
-      <c r="AI19" t="n">
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="n">
         <v>583</v>
       </c>
-      <c r="AJ19" s="2" t="n">
+      <c r="AK19" s="2" t="n">
         <v>45742</v>
       </c>
-      <c r="AK19" t="n">
+      <c r="AL19" t="n">
         <v>625</v>
       </c>
-      <c r="AL19" t="n">
+      <c r="AM19" t="n">
         <v>630</v>
       </c>
-      <c r="AM19" t="n">
+      <c r="AN19" t="n">
         <v>542</v>
       </c>
-      <c r="AN19" t="n">
+      <c r="AO19" t="n">
         <v>535</v>
       </c>
-      <c r="AO19" t="n">
+      <c r="AP19" t="n">
         <v>517</v>
       </c>
-      <c r="AP19" t="n">
+      <c r="AQ19" t="n">
         <v>550</v>
       </c>
-      <c r="AQ19" t="n">
+      <c r="AR19" t="n">
         <v>767</v>
       </c>
-      <c r="AR19" t="n">
+      <c r="AS19" t="n">
         <v>575</v>
       </c>
-      <c r="AS19" t="n">
+      <c r="AT19" t="n">
         <v>661</v>
       </c>
-      <c r="AT19" t="n">
+      <c r="AU19" t="n">
         <v>570</v>
       </c>
-      <c r="AU19" t="n">
+      <c r="AV19" t="n">
         <v>757</v>
       </c>
-      <c r="AV19" t="n">
+      <c r="AW19" t="n">
         <v>604.5</v>
       </c>
-      <c r="AW19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -3367,49 +3367,49 @@
       <c r="AH20" t="n">
         <v>585</v>
       </c>
-      <c r="AI20" t="n">
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="n">
         <v>585</v>
       </c>
-      <c r="AJ20" s="2" t="n">
+      <c r="AK20" s="2" t="n">
         <v>45741</v>
       </c>
-      <c r="AK20" t="n">
+      <c r="AL20" t="n">
         <v>623</v>
       </c>
-      <c r="AL20" t="n">
+      <c r="AM20" t="n">
         <v>650</v>
-      </c>
-      <c r="AM20" t="n">
-        <v>535</v>
       </c>
       <c r="AN20" t="n">
         <v>535</v>
       </c>
       <c r="AO20" t="n">
+        <v>535</v>
+      </c>
+      <c r="AP20" t="n">
         <v>517</v>
       </c>
-      <c r="AP20" t="n">
+      <c r="AQ20" t="n">
         <v>552</v>
       </c>
-      <c r="AQ20" t="n">
+      <c r="AR20" t="n">
         <v>767</v>
       </c>
-      <c r="AR20" t="n">
+      <c r="AS20" t="n">
         <v>573</v>
       </c>
-      <c r="AS20" t="n">
+      <c r="AT20" t="n">
         <v>659</v>
       </c>
-      <c r="AT20" t="n">
+      <c r="AU20" t="n">
         <v>572</v>
       </c>
-      <c r="AU20" t="n">
+      <c r="AV20" t="n">
         <v>757</v>
       </c>
-      <c r="AV20" t="n">
+      <c r="AW20" t="n">
         <v>603.5</v>
       </c>
-      <c r="AW20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -3512,49 +3512,49 @@
       <c r="AH21" t="n">
         <v>585</v>
       </c>
-      <c r="AI21" t="n">
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="n">
         <v>584</v>
       </c>
-      <c r="AJ21" s="2" t="n">
+      <c r="AK21" s="2" t="n">
         <v>45740</v>
       </c>
-      <c r="AK21" t="n">
+      <c r="AL21" t="n">
         <v>622</v>
       </c>
-      <c r="AL21" t="n">
+      <c r="AM21" t="n">
         <v>650</v>
-      </c>
-      <c r="AM21" t="n">
-        <v>534</v>
       </c>
       <c r="AN21" t="n">
         <v>534</v>
       </c>
       <c r="AO21" t="n">
+        <v>534</v>
+      </c>
+      <c r="AP21" t="n">
         <v>513</v>
       </c>
-      <c r="AP21" t="n">
+      <c r="AQ21" t="n">
         <v>550</v>
       </c>
-      <c r="AQ21" t="n">
+      <c r="AR21" t="n">
         <v>763</v>
       </c>
-      <c r="AR21" t="n">
+      <c r="AS21" t="n">
         <v>577</v>
       </c>
-      <c r="AS21" t="n">
+      <c r="AT21" t="n">
         <v>658</v>
       </c>
-      <c r="AT21" t="n">
+      <c r="AU21" t="n">
         <v>569</v>
       </c>
-      <c r="AU21" t="n">
+      <c r="AV21" t="n">
         <v>753</v>
       </c>
-      <c r="AV21" t="n">
+      <c r="AW21" t="n">
         <v>599.5</v>
       </c>
-      <c r="AW21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -3657,49 +3657,49 @@
       <c r="AH22" t="n">
         <v>583</v>
       </c>
-      <c r="AI22" t="n">
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="n">
         <v>584</v>
       </c>
-      <c r="AJ22" s="2" t="n">
+      <c r="AK22" s="2" t="n">
         <v>45737</v>
       </c>
-      <c r="AK22" t="n">
+      <c r="AL22" t="n">
         <v>621</v>
       </c>
-      <c r="AL22" t="n">
+      <c r="AM22" t="n">
         <v>648</v>
       </c>
-      <c r="AM22" t="n">
+      <c r="AN22" t="n">
         <v>537</v>
       </c>
-      <c r="AN22" t="n">
+      <c r="AO22" t="n">
         <v>527</v>
       </c>
-      <c r="AO22" t="n">
+      <c r="AP22" t="n">
         <v>514</v>
       </c>
-      <c r="AP22" t="n">
+      <c r="AQ22" t="n">
         <v>551</v>
       </c>
-      <c r="AQ22" t="n">
+      <c r="AR22" t="n">
         <v>763</v>
       </c>
-      <c r="AR22" t="n">
+      <c r="AS22" t="n">
         <v>576</v>
       </c>
-      <c r="AS22" t="n">
+      <c r="AT22" t="n">
         <v>657</v>
       </c>
-      <c r="AT22" t="n">
+      <c r="AU22" t="n">
         <v>570</v>
       </c>
-      <c r="AU22" t="n">
+      <c r="AV22" t="n">
         <v>753</v>
       </c>
-      <c r="AV22" t="n">
+      <c r="AW22" t="n">
         <v>592.5</v>
       </c>
-      <c r="AW22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -3802,49 +3802,49 @@
       <c r="AH23" t="n">
         <v>582</v>
       </c>
-      <c r="AI23" t="n">
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="n">
         <v>584</v>
       </c>
-      <c r="AJ23" s="2" t="n">
+      <c r="AK23" s="2" t="n">
         <v>45736</v>
       </c>
-      <c r="AK23" t="n">
+      <c r="AL23" t="n">
         <v>623</v>
       </c>
-      <c r="AL23" t="n">
+      <c r="AM23" t="n">
         <v>645</v>
       </c>
-      <c r="AM23" t="n">
+      <c r="AN23" t="n">
         <v>538</v>
       </c>
-      <c r="AN23" t="n">
+      <c r="AO23" t="n">
         <v>527</v>
       </c>
-      <c r="AO23" t="n">
+      <c r="AP23" t="n">
         <v>509</v>
       </c>
-      <c r="AP23" t="n">
+      <c r="AQ23" t="n">
         <v>548</v>
       </c>
-      <c r="AQ23" t="n">
+      <c r="AR23" t="n">
         <v>758</v>
       </c>
-      <c r="AR23" t="n">
+      <c r="AS23" t="n">
         <v>574</v>
       </c>
-      <c r="AS23" t="n">
+      <c r="AT23" t="n">
         <v>659</v>
       </c>
-      <c r="AT23" t="n">
+      <c r="AU23" t="n">
         <v>567</v>
       </c>
-      <c r="AU23" t="n">
+      <c r="AV23" t="n">
         <v>748</v>
       </c>
-      <c r="AV23" t="n">
+      <c r="AW23" t="n">
         <v>591.5</v>
       </c>
-      <c r="AW23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -3947,49 +3947,49 @@
       <c r="AH24" t="n">
         <v>583</v>
       </c>
-      <c r="AI24" t="n">
+      <c r="AI24" t="inlineStr"/>
+      <c r="AJ24" t="n">
         <v>582</v>
       </c>
-      <c r="AJ24" s="2" t="n">
+      <c r="AK24" s="2" t="n">
         <v>45735</v>
       </c>
-      <c r="AK24" t="n">
+      <c r="AL24" t="n">
         <v>617</v>
       </c>
-      <c r="AL24" t="n">
+      <c r="AM24" t="n">
         <v>645</v>
       </c>
-      <c r="AM24" t="n">
+      <c r="AN24" t="n">
         <v>537</v>
       </c>
-      <c r="AN24" t="n">
+      <c r="AO24" t="n">
         <v>529</v>
       </c>
-      <c r="AO24" t="n">
+      <c r="AP24" t="n">
         <v>502</v>
       </c>
-      <c r="AP24" t="n">
+      <c r="AQ24" t="n">
         <v>542</v>
       </c>
-      <c r="AQ24" t="n">
+      <c r="AR24" t="n">
         <v>752</v>
       </c>
-      <c r="AR24" t="n">
+      <c r="AS24" t="n">
         <v>569</v>
       </c>
-      <c r="AS24" t="n">
+      <c r="AT24" t="n">
         <v>653</v>
       </c>
-      <c r="AT24" t="n">
+      <c r="AU24" t="n">
         <v>561</v>
       </c>
-      <c r="AU24" t="n">
+      <c r="AV24" t="n">
         <v>742</v>
       </c>
-      <c r="AV24" t="n">
+      <c r="AW24" t="n">
         <v>585.5</v>
       </c>
-      <c r="AW24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -4092,49 +4092,49 @@
       <c r="AH25" t="n">
         <v>580</v>
       </c>
-      <c r="AI25" t="n">
+      <c r="AI25" t="inlineStr"/>
+      <c r="AJ25" t="n">
         <v>590</v>
       </c>
-      <c r="AJ25" s="2" t="n">
+      <c r="AK25" s="2" t="n">
         <v>45734</v>
       </c>
-      <c r="AK25" t="n">
+      <c r="AL25" t="n">
         <v>622</v>
       </c>
-      <c r="AL25" t="n">
+      <c r="AM25" t="n">
         <v>640</v>
       </c>
-      <c r="AM25" t="n">
+      <c r="AN25" t="n">
         <v>535</v>
       </c>
-      <c r="AN25" t="n">
+      <c r="AO25" t="n">
         <v>529</v>
       </c>
-      <c r="AO25" t="n">
+      <c r="AP25" t="n">
         <v>511</v>
       </c>
-      <c r="AP25" t="n">
+      <c r="AQ25" t="n">
         <v>550</v>
       </c>
-      <c r="AQ25" t="n">
+      <c r="AR25" t="n">
         <v>762</v>
       </c>
-      <c r="AR25" t="n">
+      <c r="AS25" t="n">
         <v>564</v>
       </c>
-      <c r="AS25" t="n">
+      <c r="AT25" t="n">
         <v>658</v>
       </c>
-      <c r="AT25" t="n">
+      <c r="AU25" t="n">
         <v>570</v>
       </c>
-      <c r="AU25" t="n">
+      <c r="AV25" t="n">
         <v>752</v>
       </c>
-      <c r="AV25" t="n">
+      <c r="AW25" t="n">
         <v>591.5</v>
       </c>
-      <c r="AW25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -4237,49 +4237,49 @@
       <c r="AH26" t="n">
         <v>578</v>
       </c>
-      <c r="AI26" t="n">
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="n">
         <v>600</v>
       </c>
-      <c r="AJ26" s="2" t="n">
+      <c r="AK26" s="2" t="n">
         <v>45733</v>
       </c>
-      <c r="AK26" t="n">
+      <c r="AL26" t="n">
         <v>616</v>
       </c>
-      <c r="AL26" t="n">
+      <c r="AM26" t="n">
         <v>620</v>
       </c>
-      <c r="AM26" t="n">
+      <c r="AN26" t="n">
         <v>536</v>
       </c>
-      <c r="AN26" t="n">
+      <c r="AO26" t="n">
         <v>529</v>
       </c>
-      <c r="AO26" t="n">
+      <c r="AP26" t="n">
         <v>505</v>
       </c>
-      <c r="AP26" t="n">
+      <c r="AQ26" t="n">
         <v>543</v>
       </c>
-      <c r="AQ26" t="n">
+      <c r="AR26" t="n">
         <v>756</v>
       </c>
-      <c r="AR26" t="n">
+      <c r="AS26" t="n">
         <v>568</v>
       </c>
-      <c r="AS26" t="n">
+      <c r="AT26" t="n">
         <v>652</v>
       </c>
-      <c r="AT26" t="n">
+      <c r="AU26" t="n">
         <v>563</v>
       </c>
-      <c r="AU26" t="n">
+      <c r="AV26" t="n">
         <v>746</v>
       </c>
-      <c r="AV26" t="n">
+      <c r="AW26" t="n">
         <v>588.5</v>
       </c>
-      <c r="AW26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -4382,49 +4382,49 @@
       <c r="AH27" t="n">
         <v>578</v>
       </c>
-      <c r="AI27" t="n">
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="n">
         <v>605</v>
       </c>
-      <c r="AJ27" s="2" t="n">
+      <c r="AK27" s="2" t="n">
         <v>45730</v>
       </c>
-      <c r="AK27" t="n">
+      <c r="AL27" t="n">
         <v>610</v>
       </c>
-      <c r="AL27" t="n">
+      <c r="AM27" t="n">
         <v>620</v>
       </c>
-      <c r="AM27" t="n">
+      <c r="AN27" t="n">
         <v>530</v>
       </c>
-      <c r="AN27" t="n">
+      <c r="AO27" t="n">
         <v>527</v>
       </c>
-      <c r="AO27" t="n">
+      <c r="AP27" t="n">
         <v>505</v>
       </c>
-      <c r="AP27" t="n">
+      <c r="AQ27" t="n">
         <v>543</v>
       </c>
-      <c r="AQ27" t="n">
+      <c r="AR27" t="n">
         <v>760</v>
       </c>
-      <c r="AR27" t="n">
+      <c r="AS27" t="n">
         <v>578</v>
       </c>
-      <c r="AS27" t="n">
+      <c r="AT27" t="n">
         <v>646</v>
       </c>
-      <c r="AT27" t="n">
+      <c r="AU27" t="n">
         <v>563</v>
       </c>
-      <c r="AU27" t="n">
+      <c r="AV27" t="n">
         <v>750</v>
       </c>
-      <c r="AV27" t="n">
+      <c r="AW27" t="n">
         <v>584.5</v>
       </c>
-      <c r="AW27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -4527,49 +4527,49 @@
       <c r="AH28" t="n">
         <v>578</v>
       </c>
-      <c r="AI28" t="n">
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="n">
         <v>608</v>
       </c>
-      <c r="AJ28" s="2" t="n">
+      <c r="AK28" s="2" t="n">
         <v>45729</v>
       </c>
-      <c r="AK28" t="n">
+      <c r="AL28" t="n">
         <v>613</v>
       </c>
-      <c r="AL28" t="n">
+      <c r="AM28" t="n">
         <v>620</v>
       </c>
-      <c r="AM28" t="n">
+      <c r="AN28" t="n">
         <v>529</v>
       </c>
-      <c r="AN28" t="n">
+      <c r="AO28" t="n">
         <v>531</v>
       </c>
-      <c r="AO28" t="n">
+      <c r="AP28" t="n">
         <v>511</v>
       </c>
-      <c r="AP28" t="n">
+      <c r="AQ28" t="n">
         <v>550</v>
       </c>
-      <c r="AQ28" t="n">
+      <c r="AR28" t="n">
         <v>775</v>
       </c>
-      <c r="AR28" t="n">
+      <c r="AS28" t="n">
         <v>576</v>
       </c>
-      <c r="AS28" t="n">
+      <c r="AT28" t="n">
         <v>649</v>
       </c>
-      <c r="AT28" t="n">
+      <c r="AU28" t="n">
         <v>570</v>
       </c>
-      <c r="AU28" t="n">
+      <c r="AV28" t="n">
         <v>765</v>
       </c>
-      <c r="AV28" t="n">
+      <c r="AW28" t="n">
         <v>578.5</v>
       </c>
-      <c r="AW28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -4672,49 +4672,49 @@
       <c r="AH29" t="n">
         <v>583</v>
       </c>
-      <c r="AI29" t="n">
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="n">
         <v>608</v>
       </c>
-      <c r="AJ29" s="2" t="n">
+      <c r="AK29" s="2" t="n">
         <v>45728</v>
       </c>
-      <c r="AK29" t="n">
+      <c r="AL29" t="n">
         <v>610</v>
       </c>
-      <c r="AL29" t="n">
+      <c r="AM29" t="n">
         <v>626</v>
       </c>
-      <c r="AM29" t="n">
+      <c r="AN29" t="n">
         <v>528</v>
       </c>
-      <c r="AN29" t="n">
+      <c r="AO29" t="n">
         <v>527</v>
       </c>
-      <c r="AO29" t="n">
+      <c r="AP29" t="n">
         <v>504</v>
       </c>
-      <c r="AP29" t="n">
+      <c r="AQ29" t="n">
         <v>545</v>
       </c>
-      <c r="AQ29" t="n">
+      <c r="AR29" t="n">
         <v>768</v>
       </c>
-      <c r="AR29" t="n">
+      <c r="AS29" t="n">
         <v>578</v>
       </c>
-      <c r="AS29" t="n">
+      <c r="AT29" t="n">
         <v>646</v>
       </c>
-      <c r="AT29" t="n">
+      <c r="AU29" t="n">
         <v>565</v>
       </c>
-      <c r="AU29" t="n">
+      <c r="AV29" t="n">
         <v>758</v>
       </c>
-      <c r="AV29" t="n">
+      <c r="AW29" t="n">
         <v>573.5</v>
       </c>
-      <c r="AW29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update BunkerPrices at 2025-05-09 06:59
</commit_message>
<xml_diff>
--- a/data/bunker_prices.xlsx
+++ b/data/bunker_prices.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:CP2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -673,6 +673,241 @@
           <t>Montreal*</t>
         </is>
       </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>MFSPD00</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>MFFJD00</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>MFJPD00</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>BAMFB00</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>MFSKD00</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>WKMFA00</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>MFHKD00</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>MFSHD00</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>MFZSD00</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>MFDSY00</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>MFDMB00</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>MFDKW00</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>MFDKF00</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>MFDMM00</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>MFDCL00</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>MFAGD00</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>MFDBD00</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>MFGBD00</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>MFMLD00</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>MFPRD00</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>MFRDD00</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>MFDAN00</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>MFDGT00</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>MFDHB00</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>MFDIS00</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>MFDLP00</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>MFDNV00</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>MFDPT00</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>MFLIS00</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>MFLOM00</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>MFHOD00</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>MFNYD00</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>MFLAD00</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>MFNOD00</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>MFPAD00</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>MFSED00</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>MFVAD00</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>MFBAD00</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>MFCRD00</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
+          <t>MFSAD00</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>AMFVA00</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>AMFCA00</t>
+        </is>
+      </c>
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>AMFGY00</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>AMFLB00</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>AMFMT00</t>
+        </is>
+      </c>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>AMFSF00</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>AMFMO00</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -816,6 +1051,53 @@
       <c r="AU2" t="n">
         <v>630</v>
       </c>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
+      <c r="CC2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr"/>
+      <c r="CH2" t="inlineStr"/>
+      <c r="CI2" t="inlineStr"/>
+      <c r="CJ2" t="inlineStr"/>
+      <c r="CK2" t="inlineStr"/>
+      <c r="CL2" t="inlineStr"/>
+      <c r="CM2" t="inlineStr"/>
+      <c r="CN2" t="inlineStr"/>
+      <c r="CO2" t="inlineStr"/>
+      <c r="CP2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>